<commit_message>
Add state machine updates to order items and fix bugs
</commit_message>
<xml_diff>
--- a/Vending-Items.xlsx
+++ b/Vending-Items.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>7up</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>Coca-Cola</t>
-  </si>
-  <si>
-    <t>Diet Coke</t>
   </si>
   <si>
     <t>Dr. Pepper</t>
@@ -385,11 +382,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -398,10 +393,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -449,7 +444,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -457,14 +452,6 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
         <v>2</v>
       </c>
     </row>

</xml_diff>